<commit_message>
MSE added for all networks
Error rates are correct and I have updated the same on the excel sheet.
net_3_15 is still the best model though.
</commit_message>
<xml_diff>
--- a/regression_plots.xlsx
+++ b/regression_plots.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Errors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,16 +25,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>net_3_15</t>
+  </si>
+  <si>
+    <t>Net_1_40</t>
+  </si>
+  <si>
+    <t>Net_2_10</t>
+  </si>
+  <si>
+    <t>Net_3_15</t>
+  </si>
+  <si>
+    <t>Net_3_10</t>
+  </si>
+  <si>
+    <t>Net_4_10</t>
+  </si>
+  <si>
+    <t>Net_2_5</t>
+  </si>
+  <si>
+    <t>Net_2_7</t>
+  </si>
+  <si>
+    <t>Output Scale</t>
+  </si>
+  <si>
+    <t>Error(10^-4)</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Absolute Mean Sq Error</t>
+  </si>
+  <si>
+    <t>didn’t reach convergence in 1000 iterations</t>
+  </si>
+  <si>
+    <t>Tried trainrp which did not reach convergence in 1000 iterations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -41,13 +81,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,8 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,6 +320,44 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="11811000"/>
+          <a:ext cx="4762500" cy="4762500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12192000" y="1333500"/>
           <a:ext cx="4762500" cy="4762500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -539,14 +633,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B27"/>
+  <dimension ref="B6:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="J5" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="6" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>0</v>
@@ -556,4 +655,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1">
+        <v>41551</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4.1962999999999999</v>
+      </c>
+      <c r="C3">
+        <f>B3*$B$1 / 10000</f>
+        <v>17.436046130000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5.2718999999999996</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C9" si="0">B4*$B$1 / 10000</f>
+        <v>21.905271689999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>5.0792000000000002</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>21.104583920000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4.6334</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>19.25224034</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>3.9939</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>16.595053890000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3.2755999999999998</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>13.610445559999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>3.8582999999999998</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>16.031622329999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>